<commit_message>
Removed priority on testcase level and updated tesng.xml
</commit_message>
<xml_diff>
--- a/SeleniumFramework/src/test/resources/excel/testdata.xlsx
+++ b/SeleniumFramework/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MY\SeleniumAutomationFramework\SeleniumFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MY\git\OrangeHRMAutomationFramework\SeleniumFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F6BFBC-E6CC-4636-BF70-F8E359469BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D10912-44A8-42C2-A161-830A375540FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="90">
   <si>
     <t>testname</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>updatesGeneralInformationData</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>registrationNumber</t>
@@ -633,9 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7123D11-BFD2-4C1D-B840-399C6074298E}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -664,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -714,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -770,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -820,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -876,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -926,10 +921,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -982,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -1032,10 +1027,10 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -1088,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -1138,10 +1133,10 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>7</v>
@@ -1194,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
@@ -1244,10 +1239,10 @@
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -1259,13 +1254,13 @@
         <v>56</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>57</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
         <v>58</v>
@@ -1300,25 +1295,25 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
       <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
         <v>72</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>73</v>
       </c>
-      <c r="H13" t="s">
-        <v>74</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>17</v>
@@ -1344,10 +1339,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -1359,19 +1354,19 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
         <v>76</v>
       </c>
-      <c r="G14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>17</v>
@@ -1406,16 +1401,16 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>17</v>
@@ -1450,25 +1445,25 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>17</v>

</xml_diff>